<commit_message>
Change excel template file
</commit_message>
<xml_diff>
--- a/public/template/Template_Import_Point.xlsx
+++ b/public/template/Template_Import_Point.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HCMUS-EDU\src\Classrooms-management-website\public\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_data\Classrooms-management-website\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9C4844-FCD6-4FF4-9BD9-30CFC218DD35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA332584-AAC1-49F5-A259-50EBFA14D116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4188" yWindow="1404" windowWidth="16584" windowHeight="9420" xr2:uid="{3BB9D807-3869-475C-964E-3F36CA0F5B73}"/>
+    <workbookView xWindow="5988" yWindow="1728" windowWidth="17280" windowHeight="8964" xr2:uid="{3BB9D807-3869-475C-964E-3F36CA0F5B73}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -394,7 +394,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -409,7 +409,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1</v>
+        <v>123</v>
       </c>
       <c r="B2">
         <v>100</v>
@@ -417,7 +417,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2</v>
+        <v>345</v>
       </c>
       <c r="B3">
         <v>1000</v>
@@ -425,7 +425,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="B4">
         <v>1232</v>
@@ -433,18 +433,25 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>4</v>
+        <v>30697813</v>
       </c>
       <c r="B5">
-        <v>123123</v>
+        <v>86.5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -453,7 +460,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A80EBA61DBEBAC47997BD1227BBFF84F" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4a2bb5911e9f93b0e21cdad9a75d8f76">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9d9b5332-a5d8-4d74-b69a-d1c687b97975" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="aa81d55e7a2735af0e834f88de5aac08" ns3:_="">
     <xsd:import namespace="9d9b5332-a5d8-4d74-b69a-d1c687b97975"/>
@@ -599,13 +606,23 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{822F79AB-7C51-469D-BBA3-06DFBB7D8E92}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="9d9b5332-a5d8-4d74-b69a-d1c687b97975"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA2284C4-4553-472C-99E9-F8AA8FDB4697}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -613,7 +630,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DDD0276-35B6-4B88-9546-D3E7F31A4548}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -629,20 +646,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{822F79AB-7C51-469D-BBA3-06DFBB7D8E92}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="9d9b5332-a5d8-4d74-b69a-d1c687b97975"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>